<commit_message>
mess menu added static
</commit_message>
<xml_diff>
--- a/Complaint_Form.xlsx
+++ b/Complaint_Form.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -524,6 +524,31 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Jerrygood</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>deepakverma.knp2019@gmail.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>xyz</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>xyz</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Logo added, Notice Board fixed and Complaint Form Sheet added
</commit_message>
<xml_diff>
--- a/Complaint_Form.xlsx
+++ b/Complaint_Form.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -574,6 +574,337 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Nabhya</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>nabhyakhoria@gmail.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>ABCD</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>BABACSZCascs</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Nabhya</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>nabhyakhoria@gmail.com</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Room fan not working</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Room SDS 440.
+Check asap</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>nabhyakhoria@gmail.com</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>nabhyakhoria@gmail.com</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>sadsad</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>wdqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>nabhyakhoria@gmail.com</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>nabhyakhoria@gmail.com</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>sadsad</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>wdqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>nabhyakhoria@gmail.com</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>nabhyakhoria@gmail.com</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>sadsad</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>wdqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>11</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>nabhyakhoria@gmail.com</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>nabhyakhoria@gmail.com</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>sadsad</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>wdqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>12</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Nabhya</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>nabhyakhoria@gmail.com</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Room fan not working</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Room SDS 440.
+Check asap</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>13</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Nabhya</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>nabhyakhoria@gmail.com</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Room fan not working</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Room SDS 440.
+Check asap</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>14</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Nabhya</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>nabhyakhoria@gmail.com</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Room fan not working</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Room SDS 440.
+Check asap</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>15</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Nabhya</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>nabhyakhoria@gmail.com</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Room fan not working</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Room SDS 440.
+Check asap</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>16</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Nabhya</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>nabhyakhoria@gmail.com</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Room fan not working</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Room SDS 440.
+Check asap</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>17</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Nabhya Khoria</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>nabhyakhoria@gmail.com</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Nice</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>HAt</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>18</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Shivam Singh</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>shivam@gmail.com</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>VP</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New VP </t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Final changes in mess menu
</commit_message>
<xml_diff>
--- a/Complaint_Form.xlsx
+++ b/Complaint_Form.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -905,6 +905,31 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>19</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Yash Kumar</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>yash@nfp</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>SDS 303</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Bulb not working.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>